<commit_message>
Edited files, Worked on WriteUp. Almost done, finishing up MPI.
</commit_message>
<xml_diff>
--- a/WriteUp_Data/mpi_data_avg.xlsx
+++ b/WriteUp_Data/mpi_data_avg.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\cis520\git\cis520_proj4\WriteUp_Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\git\cis520\proj4\cis520_proj4\WriteUp_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="mpi_data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -3476,16 +3476,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>409575</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4056,8 +4056,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4106,7 +4106,7 @@
         <v>76</v>
       </c>
       <c r="I2">
-        <f>(B1+B16+B31+B46+B61)/5</f>
+        <f t="shared" ref="I2:I16" si="0">(B1+B16+B31+B46+B61)/5</f>
         <v>2448511.8552000001</v>
       </c>
     </row>
@@ -4127,7 +4127,7 @@
         <v>79</v>
       </c>
       <c r="I3">
-        <f>(B2+B17+B32+B47+B62)/5</f>
+        <f t="shared" si="0"/>
         <v>1198931.8245999999</v>
       </c>
     </row>
@@ -4148,7 +4148,7 @@
         <v>80</v>
       </c>
       <c r="I4">
-        <f>(B3+B18+B33+B48+B63)/5</f>
+        <f t="shared" si="0"/>
         <v>745807.44519999996</v>
       </c>
     </row>
@@ -4169,7 +4169,7 @@
         <v>81</v>
       </c>
       <c r="I5">
-        <f>(B4+B19+B34+B49+B64)/5</f>
+        <f t="shared" si="0"/>
         <v>2430192.8931999998</v>
       </c>
     </row>
@@ -4190,7 +4190,7 @@
         <v>82</v>
       </c>
       <c r="I6">
-        <f>(B5+B20+B35+B50+B65)/5</f>
+        <f t="shared" si="0"/>
         <v>1284412.4887999999</v>
       </c>
     </row>
@@ -4211,7 +4211,7 @@
         <v>84</v>
       </c>
       <c r="I7">
-        <f>(B6+B21+B36+B51+B66)/5</f>
+        <f t="shared" si="0"/>
         <v>943385.15299999993</v>
       </c>
     </row>
@@ -4232,7 +4232,7 @@
         <v>83</v>
       </c>
       <c r="I8">
-        <f>(B7+B22+B37+B52+B67)/5</f>
+        <f t="shared" si="0"/>
         <v>450769.65619999997</v>
       </c>
     </row>
@@ -4253,7 +4253,7 @@
         <v>85</v>
       </c>
       <c r="I9">
-        <f>(B8+B23+B38+B53+B68)/5</f>
+        <f t="shared" si="0"/>
         <v>1261922.6656000002</v>
       </c>
     </row>
@@ -4274,7 +4274,7 @@
         <v>86</v>
       </c>
       <c r="I10">
-        <f>(B9+B24+B39+B54+B69)/5</f>
+        <f t="shared" si="0"/>
         <v>702071.13280000002</v>
       </c>
     </row>
@@ -4295,7 +4295,7 @@
         <v>87</v>
       </c>
       <c r="I11">
-        <f>(B10+B25+B40+B55+B70)/5</f>
+        <f t="shared" si="0"/>
         <v>405994.08799999999</v>
       </c>
     </row>
@@ -4316,7 +4316,7 @@
         <v>88</v>
       </c>
       <c r="I12">
-        <f>(B11+B26+B41+B56+B71)/5</f>
+        <f t="shared" si="0"/>
         <v>251912.24720000001</v>
       </c>
     </row>
@@ -4337,7 +4337,7 @@
         <v>89</v>
       </c>
       <c r="I13">
-        <f>(B12+B27+B42+B57+B72)/5</f>
+        <f t="shared" si="0"/>
         <v>673953.74799999991</v>
       </c>
     </row>
@@ -4358,7 +4358,7 @@
         <v>90</v>
       </c>
       <c r="I14">
-        <f>(B13+B28+B43+B58+B73)/5</f>
+        <f t="shared" si="0"/>
         <v>387103.15939999995</v>
       </c>
     </row>
@@ -4379,7 +4379,7 @@
         <v>91</v>
       </c>
       <c r="I15">
-        <f>(B14+B29+B44+B59+B74)/5</f>
+        <f t="shared" si="0"/>
         <v>257629.9768</v>
       </c>
     </row>
@@ -4400,7 +4400,7 @@
         <v>92</v>
       </c>
       <c r="I16">
-        <f>(B15+B30+B45+B60+B75)/5</f>
+        <f t="shared" si="0"/>
         <v>122586.4926</v>
       </c>
     </row>

</xml_diff>